<commit_message>
Uploading get data codes
</commit_message>
<xml_diff>
--- a/config/spec.xlsx
+++ b/config/spec.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/381604333a3d9f7b/Documentos/FGV/Monografia/DeterminantsofParticipation/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="407" documentId="8_{9C97BED5-9F04-42D7-855F-2785861323AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFEC32DB-0CB6-419F-9B74-0E08DC8F1E04}"/>
+  <xr:revisionPtr revIDLastSave="417" documentId="8_{9C97BED5-9F04-42D7-855F-2785861323AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17F51398-F4EE-4A2F-B5AD-CAA6FC87A7C4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="756" xr2:uid="{C616E66A-E69A-487A-B090-6C78F2086441}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="756" xr2:uid="{C616E66A-E69A-487A-B090-6C78F2086441}"/>
   </bookViews>
   <sheets>
     <sheet name="asec" sheetId="1" r:id="rId1"/>
-    <sheet name="jolts_industry" sheetId="2" r:id="rId2"/>
+    <sheet name="old_vars" sheetId="3" r:id="rId2"/>
+    <sheet name="jolts_industry" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">asec!$A$1:$C$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">asec!$A$1:$C$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="242">
   <si>
     <t>Name</t>
   </si>
@@ -135,9 +136,6 @@
     <t>HPRES_MORT</t>
   </si>
   <si>
-    <t>HEFAMINC</t>
-  </si>
-  <si>
     <t>Renda Familiar</t>
   </si>
   <si>
@@ -276,12 +274,6 @@
     <t>HINTVAL</t>
   </si>
   <si>
-    <t>Renda Domiciliar Assistência Social</t>
-  </si>
-  <si>
-    <t>HPAWVAL</t>
-  </si>
-  <si>
     <t>Renda Domiciliar Pensão</t>
   </si>
   <si>
@@ -772,6 +764,9 @@
   </si>
   <si>
     <t>GMSTCEN</t>
+  </si>
+  <si>
+    <t>HTOTVAL</t>
   </si>
 </sst>
 </file>
@@ -1164,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771C8B08-53F6-49FC-9B9C-8D2D536EA572}">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1185,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1196,84 +1191,84 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1284,7 +1279,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1295,7 +1290,7 @@
         <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1306,444 +1301,444 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
         <v>39</v>
       </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
         <v>37</v>
       </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
         <v>55</v>
       </c>
-      <c r="B16" t="s">
-        <v>56</v>
-      </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
         <v>64</v>
       </c>
-      <c r="B17" t="s">
-        <v>65</v>
-      </c>
       <c r="C17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
         <v>66</v>
       </c>
-      <c r="B19" t="s">
-        <v>67</v>
-      </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="B20" t="s">
-        <v>69</v>
-      </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
         <v>70</v>
       </c>
-      <c r="B21" t="s">
-        <v>71</v>
-      </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
         <v>72</v>
       </c>
-      <c r="B22" t="s">
-        <v>73</v>
-      </c>
       <c r="C22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>241</v>
       </c>
       <c r="C23" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C24" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
         <v>74</v>
       </c>
-      <c r="B26" t="s">
-        <v>75</v>
-      </c>
       <c r="C26" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
         <v>60</v>
       </c>
-      <c r="B27" t="s">
-        <v>61</v>
-      </c>
       <c r="C27" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" t="s">
         <v>76</v>
       </c>
-      <c r="B28" t="s">
-        <v>77</v>
-      </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
         <v>78</v>
       </c>
-      <c r="B30" t="s">
-        <v>79</v>
-      </c>
       <c r="C30" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="C35" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B43" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="C44" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B45" t="s">
-        <v>97</v>
+        <v>28</v>
       </c>
       <c r="C45" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C47" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C48" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="C50" t="s">
-        <v>106</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>178</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>179</v>
       </c>
       <c r="C51" t="s">
-        <v>151</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
+        <v>182</v>
+      </c>
+      <c r="B52" t="s">
         <v>181</v>
-      </c>
-      <c r="B52" t="s">
-        <v>182</v>
       </c>
       <c r="C52" t="s">
         <v>183</v>
@@ -1751,54 +1746,54 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>242</v>
+        <v>184</v>
       </c>
       <c r="B53" t="s">
-        <v>243</v>
+        <v>185</v>
       </c>
       <c r="C53" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B54" t="s">
-        <v>184</v>
-      </c>
-      <c r="C54" t="s">
-        <v>186</v>
+        <v>188</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>240</v>
+        <v>189</v>
       </c>
       <c r="B55" t="s">
-        <v>241</v>
-      </c>
-      <c r="C55" t="s">
-        <v>186</v>
+        <v>190</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B56" t="s">
-        <v>188</v>
-      </c>
-      <c r="C56" t="s">
-        <v>189</v>
+        <v>192</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B57" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1806,10 +1801,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B58" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1817,10 +1812,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B59" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1828,10 +1823,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B60" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1839,10 +1834,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B61" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1850,10 +1845,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B62" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1861,10 +1856,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B63" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1872,10 +1867,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B64" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1883,10 +1878,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B65" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1894,10 +1889,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B66" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1905,10 +1900,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B67" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1916,10 +1911,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B68" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1927,10 +1922,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B69" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1938,10 +1933,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B70" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1949,43 +1944,43 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B71" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B72" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B73" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B74" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C74">
         <v>3</v>
@@ -1993,21 +1988,21 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B75" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C75">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B76" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="C76">
         <v>3</v>
@@ -2015,63 +2010,30 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B77" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C77">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B78" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C78">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>234</v>
-      </c>
-      <c r="B79" t="s">
-        <v>239</v>
-      </c>
-      <c r="C79">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
-        <v>235</v>
-      </c>
-      <c r="B80" t="s">
-        <v>236</v>
-      </c>
-      <c r="C80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
-        <v>238</v>
-      </c>
-      <c r="B81" t="s">
-        <v>237</v>
-      </c>
-      <c r="C81">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C51" xr:uid="{771C8B08-53F6-49FC-9B9C-8D2D536EA572}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C51">
-      <sortCondition ref="B1:B51"/>
+  <autoFilter ref="A1:C50" xr:uid="{771C8B08-53F6-49FC-9B9C-8D2D536EA572}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C50">
+      <sortCondition ref="B1:B50"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2079,6 +2041,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{696B70DC-D974-4C42-B58C-9BB9E3A42C45}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE98301-FC03-4B74-A17D-63D37E655BE7}">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -2095,16 +2094,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2112,7 +2111,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2120,13 +2119,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C3">
         <v>110099</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2134,13 +2133,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C4">
         <v>230000</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2148,13 +2147,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C5">
         <v>300000</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2162,13 +2161,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2176,13 +2175,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C7">
         <v>480099</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2190,13 +2189,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C8">
         <v>510000</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2204,13 +2203,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C9">
         <v>510099</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2218,13 +2217,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C10">
         <v>540099</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2232,13 +2231,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C11">
         <v>600000</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2246,13 +2245,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C12">
         <v>700000</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2260,13 +2259,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C13">
         <v>810000</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2274,13 +2273,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C14" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2288,7 +2287,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>